<commit_message>
adjusted summary of isotopic assignments
</commit_message>
<xml_diff>
--- a/output/IsotopeAssignment_Tables.xlsx
+++ b/output/IsotopeAssignment_Tables.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="98" documentId="8_{B42A1943-A9CE-4CF4-AD3C-820061E5FADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FFC537A-D9EE-4275-8332-1CBD5170B09A}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5D21C7A2-26BC-491D-AB66-107084B0D458}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5D21C7A2-26BC-491D-AB66-107084B0D458}"/>
   </bookViews>
   <sheets>
     <sheet name="Table11_SampleSize" sheetId="4" r:id="rId1"/>
@@ -928,7 +928,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCE4BA5C-1840-4AFF-96BF-357DC86074E0}">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>

</xml_diff>